<commit_message>
update in case the phone number is wrong
</commit_message>
<xml_diff>
--- a/Contatos.xlsx
+++ b/Contatos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a204c6e7845b6cdb/Área de Trabalho/Jonathan/UDESC/algoritmo/python/Automação para envio de cardapios/Automazap/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a204c6e7845b6cdb/Área de Trabalho/Jonathan/Automazap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{1AE800CF-B3A2-435E-AEF4-3308DF48D731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AEE9197-A615-4BDB-AA36-1A3E1383AD07}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{1AE800CF-B3A2-435E-AEF4-3308DF48D731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8719E17-E806-4DE8-B4D2-F27B939DF676}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F81C85CE-3BCD-4B33-8C8B-0A39913C8743}"/>
   </bookViews>
@@ -46,8 +46,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -75,10 +83,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,7 +409,7 @@
   <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,7 +445,7 @@
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>

</xml_diff>